<commit_message>
Deploying to gh-pages from @ matthewdlang18/macroeconomics-course-website@65a66ca5f21f2e68197b299361da1869bc536acb 🚀
</commit_message>
<xml_diff>
--- a/activities/activity3/data/Discussion Activity 3, AI Response.xlsx
+++ b/activities/activity3/data/Discussion Activity 3, AI Response.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattlang/Cursor/macroeconomics-course-website/activities/activity3/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EDD709-FF61-464A-97DD-1CE5148E9E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29260" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>Indicator</t>
   </si>
@@ -56,32 +65,78 @@
   </si>
   <si>
     <t>S&amp;P 500</t>
+  </si>
+  <si>
+    <t>12-Month GDP Growth</t>
+  </si>
+  <si>
+    <t>24-Month GDP Growth</t>
+  </si>
+  <si>
+    <t>Recession Probability</t>
+  </si>
+  <si>
+    <t>Weak Growth</t>
+  </si>
+  <si>
+    <t>Moderate Growth</t>
+  </si>
+  <si>
+    <t>Severe Contraction</t>
+  </si>
+  <si>
+    <t>Mild Contraction</t>
+  </si>
+  <si>
+    <t>Strong Growth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="&quot;Aptos Narrow&quot;"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -90,42 +145,48 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -315,23 +376,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AM12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.25"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:39" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -353,12 +420,24 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="H1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -386,200 +465,458 @@
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:39" ht="16">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="F2" s="3">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="G2" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6">
+        <v>5</v>
+      </c>
+      <c r="I2" s="6">
+        <v>50</v>
+      </c>
+      <c r="J2" s="6">
+        <v>20</v>
+      </c>
+      <c r="K2" s="6">
+        <v>20</v>
+      </c>
+      <c r="L2" s="6">
+        <v>30</v>
+      </c>
+      <c r="M2" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" ht="16">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F3" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="G3" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>5</v>
+      </c>
+      <c r="H3" s="6">
+        <v>5</v>
+      </c>
+      <c r="I3" s="6">
+        <v>10</v>
+      </c>
+      <c r="J3" s="6">
+        <v>20</v>
+      </c>
+      <c r="K3" s="6">
+        <v>20</v>
+      </c>
+      <c r="L3" s="6">
+        <v>5</v>
+      </c>
+      <c r="M3" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" ht="16">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C4" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="E4" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F4" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="G4" s="3">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>10</v>
+      </c>
+      <c r="H4" s="6">
+        <v>30</v>
+      </c>
+      <c r="I4" s="6">
+        <v>10</v>
+      </c>
+      <c r="J4" s="6">
+        <v>20</v>
+      </c>
+      <c r="K4" s="6">
+        <v>20</v>
+      </c>
+      <c r="L4" s="6">
+        <v>5</v>
+      </c>
+      <c r="M4" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" ht="16">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="E5" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="F5" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="G5" s="3">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6">
+        <v>15</v>
+      </c>
+      <c r="I5" s="6">
+        <v>10</v>
+      </c>
+      <c r="J5" s="6">
+        <v>10</v>
+      </c>
+      <c r="K5" s="6">
+        <v>10</v>
+      </c>
+      <c r="L5" s="6">
+        <v>10</v>
+      </c>
+      <c r="M5" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" ht="16">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="E6" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G6" s="3">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>20</v>
+      </c>
+      <c r="H6" s="6">
+        <v>10</v>
+      </c>
+      <c r="I6" s="6">
+        <v>5</v>
+      </c>
+      <c r="J6" s="6">
+        <v>10</v>
+      </c>
+      <c r="K6" s="6">
+        <v>10</v>
+      </c>
+      <c r="L6" s="6">
+        <v>10</v>
+      </c>
+      <c r="M6" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" ht="16">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E7" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="F7" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G7" s="3">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>20</v>
+      </c>
+      <c r="H7" s="6">
+        <v>5</v>
+      </c>
+      <c r="I7" s="6">
+        <v>5</v>
+      </c>
+      <c r="J7" s="6">
+        <v>5</v>
+      </c>
+      <c r="K7" s="6">
+        <v>5</v>
+      </c>
+      <c r="L7" s="6">
+        <v>15</v>
+      </c>
+      <c r="M7" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" ht="16">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E8" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="F8" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G8" s="3">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>10</v>
+      </c>
+      <c r="H8" s="6">
+        <v>20</v>
+      </c>
+      <c r="I8" s="6">
+        <v>5</v>
+      </c>
+      <c r="J8" s="6">
+        <v>5</v>
+      </c>
+      <c r="K8" s="6">
+        <v>5</v>
+      </c>
+      <c r="L8" s="6">
+        <v>15</v>
+      </c>
+      <c r="M8" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" ht="16">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D9" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="E9" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G9" s="3">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="H9" s="6">
+        <v>10</v>
+      </c>
+      <c r="I9" s="6">
+        <v>5</v>
+      </c>
+      <c r="J9" s="6">
+        <v>10</v>
+      </c>
+      <c r="K9" s="6">
+        <v>10</v>
+      </c>
+      <c r="L9" s="6">
+        <v>10</v>
+      </c>
+      <c r="M9" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>92</v>
+      </c>
+      <c r="D12">
+        <v>89</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>94</v>
+      </c>
+      <c r="G12">
+        <v>68</v>
+      </c>
+      <c r="H12">
+        <v>50</v>
+      </c>
+      <c r="I12">
+        <v>25</v>
+      </c>
+      <c r="J12">
+        <v>16</v>
+      </c>
+      <c r="K12">
+        <v>66</v>
+      </c>
+      <c r="L12">
+        <v>45</v>
+      </c>
+      <c r="M12">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>